<commit_message>
New version 2020 of Friedrich Longin Lectures
</commit_message>
<xml_diff>
--- a/Data_Durum_students.xlsx
+++ b/Data_Durum_students.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Vorlesung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Vorlesung\Selectiongain\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11790" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11790" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Group 1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="91">
   <si>
     <t>All costs are in yield plot equivalents, e.g. 1 yield plot = 30€</t>
   </si>
@@ -116,30 +116,18 @@
     <t>cross</t>
   </si>
   <si>
-    <t>Year 2 - summer + winter</t>
-  </si>
-  <si>
     <t>DH production</t>
   </si>
   <si>
-    <t>Year 3- summer + winter</t>
-  </si>
-  <si>
     <t>Year 4 - summer</t>
   </si>
   <si>
-    <t>DH nursery</t>
-  </si>
-  <si>
     <t>Year 5 - summer</t>
   </si>
   <si>
     <t>First yield test</t>
   </si>
   <si>
-    <t>Year 6 - summer</t>
-  </si>
-  <si>
     <t>Second yield test</t>
   </si>
   <si>
@@ -282,6 +270,36 @@
   </si>
   <si>
     <t>if number of N1 &lt; 100 we have to think about extra trials for recalibration of GS accuracy</t>
+  </si>
+  <si>
+    <t>3; 4</t>
+  </si>
+  <si>
+    <t>Cost to produce 1 line with enough seed for nursery observation and multiplication of seeds</t>
+  </si>
+  <si>
+    <t>line prod</t>
+  </si>
+  <si>
+    <t>nursery</t>
+  </si>
+  <si>
+    <t>Year 2 - summer + winter (F1 + F2)</t>
+  </si>
+  <si>
+    <t>Year 3- summer + winter (F3 + F4)</t>
+  </si>
+  <si>
+    <t>Year 4 - summer (F5)</t>
+  </si>
+  <si>
+    <t>Year 5 - summer (F6)</t>
+  </si>
+  <si>
+    <t>Year 6 - summer (F7)</t>
+  </si>
+  <si>
+    <t>nursery + GS</t>
   </si>
 </sst>
 </file>
@@ -372,7 +390,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -384,6 +402,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -666,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C48"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:B38"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,15 +715,15 @@
         <v>4</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>82</v>
       </c>
       <c r="B5" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -794,7 +813,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -883,7 +902,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B27" s="4">
         <v>5</v>
@@ -926,42 +945,42 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>29</v>
+        <v>85</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>86</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>33</v>
+        <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>34</v>
+        <v>88</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>89</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -969,12 +988,12 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>26</v>
@@ -990,34 +1009,34 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>29</v>
+        <v>85</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>31</v>
+        <v>86</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>34</v>
+        <v>88</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -1032,8 +1051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C46"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1062,15 +1081,15 @@
         <v>4</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="4">
-        <v>2</v>
+      <c r="B5" s="11" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1160,7 +1179,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -1249,7 +1268,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B27" s="4">
         <v>5</v>
@@ -1280,10 +1299,10 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -1296,34 +1315,34 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -1331,15 +1350,15 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -1352,30 +1371,31 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>30</v>
+      </c>
+      <c r="B46" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1383,7 +1403,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D49"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
@@ -1413,7 +1433,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1437,12 +1457,12 @@
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B8" s="4">
         <v>1</v>
@@ -1517,7 +1537,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1624,13 +1644,13 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B32" s="6"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>28</v>
@@ -1638,50 +1658,50 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1689,18 +1709,18 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B42" s="6"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>28</v>
@@ -1708,45 +1728,45 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
@@ -1761,7 +1781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -1784,58 +1804,58 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" t="s">
         <v>77</v>
       </c>
-      <c r="C1" t="s">
-        <v>81</v>
-      </c>
       <c r="D1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" t="s">
         <v>66</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>67</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>68</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
         <v>69</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N1" t="s">
         <v>70</v>
       </c>
-      <c r="K1" t="s">
+      <c r="O1" t="s">
         <v>71</v>
       </c>
-      <c r="L1" t="s">
+      <c r="P1" t="s">
         <v>72</v>
       </c>
-      <c r="M1" t="s">
-        <v>73</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>74</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>75</v>
-      </c>
-      <c r="P1" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>78</v>
-      </c>
-      <c r="R1" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>